<commit_message>
gif updates, map bottom scroll update
</commit_message>
<xml_diff>
--- a/images/institutional_sites_metadata.xlsx
+++ b/images/institutional_sites_metadata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AC0E04-C187-4D12-B956-784B4E674B0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB6B1BB-BEE3-40CA-BEA3-3695BCEC79E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -280,15 +280,9 @@
     <t>15% Penetration Capacity (MW)</t>
   </si>
   <si>
-    <t>Existing solar generation (MW)</t>
-  </si>
-  <si>
     <t>Total rooftop area (sqft) of institutional site</t>
   </si>
   <si>
-    <t>Suitable rooftop area (sqft) suitable for solar</t>
-  </si>
-  <si>
     <t>Total parking lot area (sqft)</t>
   </si>
   <si>
@@ -332,6 +326,12 @@
   </si>
   <si>
     <t>Total residential electricity usage (kWh) by renter-occupied household within census block group (UCLA Energy Atlas)</t>
+  </si>
+  <si>
+    <t>Existing in front of the meter solar generation (MW)</t>
+  </si>
+  <si>
+    <t>Total rooftop area (sqft) of institutional site considered suitable for solar PV</t>
   </si>
 </sst>
 </file>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -788,7 +788,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -796,7 +796,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -804,7 +804,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -812,7 +812,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -820,7 +820,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -828,7 +828,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -836,7 +836,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -844,7 +844,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -852,7 +852,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -860,7 +860,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -1004,7 +1004,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -1012,7 +1012,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -1020,7 +1020,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -1028,7 +1028,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -1036,7 +1036,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -1044,7 +1044,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -1052,7 +1052,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -1060,7 +1060,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
excel download and metadata updates
</commit_message>
<xml_diff>
--- a/images/institutional_sites_metadata.xlsx
+++ b/images/institutional_sites_metadata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB6B1BB-BEE3-40CA-BEA3-3695BCEC79E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46445416-B983-4B5C-8CD4-13F5B8CA4527}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Column Name</t>
   </si>
@@ -181,12 +181,6 @@
     <t>sufficient_capacity</t>
   </si>
   <si>
-    <t>numeric ID set by CARTODB</t>
-  </si>
-  <si>
-    <t>Distribution circuit name defined by Southern California Edison (SCE)</t>
-  </si>
-  <si>
     <t>Existing generation connected to the distribution circuit (MW)</t>
   </si>
   <si>
@@ -262,12 +256,6 @@
     <t>CalEnviroScreen 3.0 Percentile</t>
   </si>
   <si>
-    <t>Substation name defined by Southern California Edison (SCE)</t>
-  </si>
-  <si>
-    <t>System name defined by Southern California Edison (SCE)</t>
-  </si>
-  <si>
     <t>Projected load (MW)</t>
   </si>
   <si>
@@ -277,9 +265,6 @@
     <t>Maximum remaining capacity (MW)</t>
   </si>
   <si>
-    <t>15% Penetration Capacity (MW)</t>
-  </si>
-  <si>
     <t>Total rooftop area (sqft) of institutional site</t>
   </si>
   <si>
@@ -289,21 +274,6 @@
     <t>Suitable parking lot area (sqft) suitable for solar</t>
   </si>
   <si>
-    <t>Low level estimate of available parking lot area solar PV generation capacity potential (MW)</t>
-  </si>
-  <si>
-    <t>High level estimate of available parking lot area solar PV generation capacity potential (MW)</t>
-  </si>
-  <si>
-    <t>Rooftop solar generation capacity potential (MW)</t>
-  </si>
-  <si>
-    <t>Combined total of the low estimate of parking lot generation potential and rooftop solar generation capacity potential (MW)</t>
-  </si>
-  <si>
-    <t>Combined total of the high estimate of parking lot generation potential and rooftop solar generation capacity potential (MW)</t>
-  </si>
-  <si>
     <t>Estimate of households within census block group where total electricity usage could be offset by the low estimate combined solar potential</t>
   </si>
   <si>
@@ -328,10 +298,46 @@
     <t>Total residential electricity usage (kWh) by renter-occupied household within census block group (UCLA Energy Atlas)</t>
   </si>
   <si>
-    <t>Existing in front of the meter solar generation (MW)</t>
-  </si>
-  <si>
     <t>Total rooftop area (sqft) of institutional site considered suitable for solar PV</t>
+  </si>
+  <si>
+    <t>numeric ID automatically set by CARTODB</t>
+  </si>
+  <si>
+    <t>site_id</t>
+  </si>
+  <si>
+    <t>Site ID corresponding to the map pop-up information for Eligible Sites</t>
+  </si>
+  <si>
+    <t>Nearest distribution circuit, name defined by Southern California Edison (SCE)</t>
+  </si>
+  <si>
+    <t>Substation name defined by Southern California Edison (SCE), linked by nearest distribution circuit</t>
+  </si>
+  <si>
+    <t>System name defined by Southern California Edison (SCE), linked by nearest distribution circuit</t>
+  </si>
+  <si>
+    <t>15% Penetration Capacity (MW-AC)</t>
+  </si>
+  <si>
+    <t>Existing in front of the meter solar generation (MW-AC)</t>
+  </si>
+  <si>
+    <t>Rooftop solar generation capacity potential (MW-AC)</t>
+  </si>
+  <si>
+    <t>Low level estimate of available parking lot area solar PV generation capacity potential (MW-AC)</t>
+  </si>
+  <si>
+    <t>High level estimate of available parking lot area solar PV generation capacity potential (MW-AC)</t>
+  </si>
+  <si>
+    <t>Combined total of the low estimate of parking lot generation potential and rooftop solar generation capacity potential (MW-AC)</t>
+  </si>
+  <si>
+    <t>Combined total of the high estimate of parking lot generation potential and rooftop solar generation capacity potential (MW-AC)</t>
   </si>
 </sst>
 </file>
@@ -382,7 +388,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -393,6 +418,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A6F866A3-FD1D-4AFD-B623-842C5D79BA10}" name="Table1" displayName="Table1" ref="A1:B53" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:B53" xr:uid="{34BE8A5B-FA84-4A8B-84CD-6F150574ECAF}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{5BB3DEBD-1C7A-40F4-87D1-F8471D0363D2}" name="Column Name"/>
+    <tableColumn id="2" xr3:uid="{AA25CDB0-24D0-4ECE-A752-7D9BD85A06E7}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -658,19 +694,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.08984375" customWidth="1"/>
+    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="140.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,416 +715,427 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>47</v>
-      </c>
-      <c r="B47" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>